<commit_message>
base code - needs refactoring but works
</commit_message>
<xml_diff>
--- a/data/MsiaAccidentCases.xlsx
+++ b/data/MsiaAccidentCases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTECH\projects\GohYangMiang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\githome\ivarunkumar\KE5205-TextMining-CA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="439">
   <si>
     <t>Title Case</t>
   </si>
@@ -1338,15 +1338,12 @@
   </si>
   <si>
     <t xml:space="preserve">Cause </t>
-  </si>
-  <si>
-    <t>TEST DATA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1836,12 +1833,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2164,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C240"/>
+  <dimension ref="A1:C236"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184:XFD187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3409,7 +3405,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="113" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>429</v>
       </c>
@@ -3519,7 +3515,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="123" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>429</v>
       </c>
@@ -3563,7 +3559,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>430</v>
       </c>
@@ -3684,7 +3680,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="138" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>430</v>
       </c>
@@ -4190,188 +4186,224 @@
         <v>328</v>
       </c>
     </row>
-    <row r="184" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A186" s="4" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>36</v>
+      </c>
+      <c r="B184" t="s">
+        <v>329</v>
+      </c>
+      <c r="C184" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>430</v>
+      </c>
+      <c r="B185" t="s">
+        <v>331</v>
+      </c>
+      <c r="C185" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>429</v>
+      </c>
+      <c r="B186" t="s">
+        <v>334</v>
+      </c>
+      <c r="C186" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>432</v>
+      </c>
+      <c r="B187" t="s">
+        <v>337</v>
+      </c>
+      <c r="C187" t="s">
+        <v>338</v>
+      </c>
+    </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>36</v>
+        <v>432</v>
       </c>
       <c r="B188" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="C188" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B189" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="C189" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B190" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="C190" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B191" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="C191" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B192" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="C192" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B193" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="C193" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B194" t="s">
-        <v>344</v>
+        <v>28</v>
       </c>
       <c r="C194" t="s">
-        <v>345</v>
+        <v>353</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B195" t="s">
-        <v>346</v>
+        <v>28</v>
       </c>
       <c r="C195" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B196" t="s">
-        <v>349</v>
+        <v>256</v>
       </c>
       <c r="C196" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B197" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C197" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B198" t="s">
-        <v>28</v>
+        <v>359</v>
       </c>
       <c r="C198" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B199" t="s">
-        <v>28</v>
+        <v>362</v>
       </c>
       <c r="C199" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B200" t="s">
-        <v>256</v>
+        <v>364</v>
       </c>
       <c r="C200" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B201" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="C201" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B202" t="s">
-        <v>359</v>
+        <v>28</v>
       </c>
       <c r="C202" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B203" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="C203" t="s">
-        <v>363</v>
+        <v>369</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -4379,10 +4411,10 @@
         <v>432</v>
       </c>
       <c r="B204" t="s">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="C204" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -4390,43 +4422,43 @@
         <v>432</v>
       </c>
       <c r="B205" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C205" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B206" t="s">
-        <v>28</v>
+        <v>374</v>
       </c>
       <c r="C206" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B207" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
       <c r="C207" t="s">
-        <v>369</v>
+        <v>377</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B208" t="s">
-        <v>370</v>
+        <v>378</v>
       </c>
       <c r="C208" t="s">
-        <v>371</v>
+        <v>379</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -4434,10 +4466,10 @@
         <v>432</v>
       </c>
       <c r="B209" t="s">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="C209" t="s">
-        <v>373</v>
+        <v>381</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -4445,32 +4477,32 @@
         <v>434</v>
       </c>
       <c r="B210" t="s">
-        <v>374</v>
+        <v>382</v>
       </c>
       <c r="C210" t="s">
-        <v>375</v>
+        <v>383</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B211" t="s">
-        <v>376</v>
+        <v>384</v>
       </c>
       <c r="C211" t="s">
-        <v>377</v>
+        <v>385</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B212" t="s">
-        <v>378</v>
+        <v>272</v>
       </c>
       <c r="C212" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -4478,98 +4510,98 @@
         <v>432</v>
       </c>
       <c r="B213" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C213" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B214" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="C214" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B215" t="s">
-        <v>384</v>
+        <v>272</v>
       </c>
       <c r="C215" t="s">
-        <v>385</v>
+        <v>391</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B216" t="s">
-        <v>272</v>
+        <v>392</v>
       </c>
       <c r="C216" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B217" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="C217" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B218" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="C218" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B219" t="s">
-        <v>272</v>
+        <v>398</v>
       </c>
       <c r="C219" t="s">
-        <v>391</v>
+        <v>399</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B220" t="s">
-        <v>392</v>
+        <v>400</v>
       </c>
       <c r="C220" t="s">
-        <v>393</v>
+        <v>401</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="B221" t="s">
-        <v>394</v>
+        <v>402</v>
       </c>
       <c r="C221" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -4577,76 +4609,76 @@
         <v>434</v>
       </c>
       <c r="B222" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="C222" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B223" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="C223" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B224" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="C224" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B225" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="C225" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="B226" t="s">
-        <v>384</v>
+        <v>409</v>
       </c>
       <c r="C226" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B227" t="s">
-        <v>405</v>
+        <v>272</v>
       </c>
       <c r="C227" t="s">
-        <v>406</v>
+        <v>412</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>430</v>
+        <v>108</v>
       </c>
       <c r="B228" t="s">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="C228" t="s">
-        <v>408</v>
+        <v>414</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -4654,130 +4686,86 @@
         <v>429</v>
       </c>
       <c r="B229" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="C229" t="s">
-        <v>410</v>
+        <v>416</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B230" t="s">
-        <v>409</v>
+        <v>272</v>
       </c>
       <c r="C230" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B231" t="s">
-        <v>272</v>
+        <v>418</v>
       </c>
       <c r="C231" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>108</v>
+        <v>435</v>
       </c>
       <c r="B232" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="C232" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="B233" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C233" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B234" t="s">
-        <v>272</v>
+        <v>424</v>
       </c>
       <c r="C234" t="s">
-        <v>417</v>
+        <v>425</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B235" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="C235" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="B236" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="C236" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A237" t="s">
-        <v>434</v>
-      </c>
-      <c r="B237" t="s">
-        <v>422</v>
-      </c>
-      <c r="C237" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A238" t="s">
-        <v>429</v>
-      </c>
-      <c r="B238" t="s">
-        <v>424</v>
-      </c>
-      <c r="C238" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A239" t="s">
-        <v>429</v>
-      </c>
-      <c r="B239" t="s">
-        <v>424</v>
-      </c>
-      <c r="C239" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A240" t="s">
-        <v>429</v>
-      </c>
-      <c r="B240" t="s">
-        <v>427</v>
-      </c>
-      <c r="C240" t="s">
         <v>428</v>
       </c>
     </row>

</xml_diff>